<commit_message>
updated templates to fix references bugs
</commit_message>
<xml_diff>
--- a/xls/templates/deadline-driven-template.xlsx
+++ b/xls/templates/deadline-driven-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toddcullen/Projects/remarkably/xls/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4336CA5F-FC5A-004C-8F10-2AB4B28D8C9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFF9DB9-8A2B-174A-B728-025123830A08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="38400" windowHeight="21060" activeTab="5" xr2:uid="{37D2F886-AD7C-B54B-8546-6E8B72F70745}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="38400" windowHeight="21060" activeTab="7" xr2:uid="{37D2F886-AD7C-B54B-8546-6E8B72F70745}"/>
   </bookViews>
   <sheets>
     <sheet name="CONSTANTS" sheetId="12" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="215">
   <si>
     <t>Start Date</t>
   </si>
@@ -366,9 +366,6 @@
     <t>spreadsheet_version</t>
   </si>
   <si>
-    <t>run_rate_model</t>
-  </si>
-  <si>
     <t>LEASING</t>
   </si>
   <si>
@@ -661,6 +658,33 @@
   </si>
   <si>
     <t>Ret Setup Cost</t>
+  </si>
+  <si>
+    <t>deadline_model</t>
+  </si>
+  <si>
+    <t>Acq DC</t>
+  </si>
+  <si>
+    <t>Acq LE</t>
+  </si>
+  <si>
+    <t>Acq MI</t>
+  </si>
+  <si>
+    <t>Acq RB</t>
+  </si>
+  <si>
+    <t>Ret DC</t>
+  </si>
+  <si>
+    <t>Ret LE</t>
+  </si>
+  <si>
+    <t>Ret MI</t>
+  </si>
+  <si>
+    <t>Ret RB</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1140,10 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="7" fillId="13" borderId="0" xfId="15" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="14"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="18"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="19"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="11" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1124,6 +1151,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
@@ -1177,21 +1216,8 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="18"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="19"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1529,7 +1555,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1539,25 +1565,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="67" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="67" t="s">
         <v>190</v>
       </c>
-      <c r="B1" s="88" t="s">
+      <c r="C1" s="67" t="s">
         <v>191</v>
-      </c>
-      <c r="C1" s="88" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1565,18 +1591,18 @@
         <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1604,7 +1630,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B1">
         <v>12</v>
@@ -1612,7 +1638,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2">
         <f>B1-2</f>
@@ -1653,7 +1679,7 @@
       <c r="A1" s="28"/>
       <c r="B1" s="28"/>
       <c r="C1" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D1" s="30"/>
       <c r="E1" s="30"/>
@@ -1664,24 +1690,24 @@
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
       <c r="L1" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M1" s="32"/>
       <c r="N1" s="32"/>
       <c r="O1" s="32"/>
       <c r="P1" s="33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q1" s="34"/>
       <c r="R1" s="34"/>
       <c r="S1" s="35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T1" s="36"/>
       <c r="U1" s="36"/>
       <c r="V1" s="36"/>
       <c r="W1" s="37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="X1" s="38"/>
       <c r="Y1" s="38"/>
@@ -1695,37 +1721,37 @@
         <v>1</v>
       </c>
       <c r="C2" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="E2" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="F2" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="G2" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="H2" s="41" t="s">
         <v>118</v>
-      </c>
-      <c r="H2" s="41" t="s">
-        <v>119</v>
       </c>
       <c r="I2" s="41" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="K2" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="L2" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="M2" s="41" t="s">
         <v>122</v>
-      </c>
-      <c r="M2" s="41" t="s">
-        <v>123</v>
       </c>
       <c r="N2" s="41" t="s">
         <v>16</v>
@@ -1740,31 +1766,31 @@
         <v>88</v>
       </c>
       <c r="R2" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="S2" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="S2" s="42" t="s">
+      <c r="T2" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="T2" s="43" t="s">
+      <c r="U2" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="U2" s="43" t="s">
+      <c r="V2" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="V2" s="43" t="s">
+      <c r="W2" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="W2" s="42" t="s">
+      <c r="X2" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="X2" s="43" t="s">
+      <c r="Y2" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="Y2" s="43" t="s">
+      <c r="Z2" s="43" t="s">
         <v>131</v>
-      </c>
-      <c r="Z2" s="43" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -18512,30 +18538,30 @@
       <c r="A1" s="47"/>
       <c r="B1" s="47"/>
       <c r="C1" s="51" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
       <c r="G1" s="51"/>
       <c r="H1" s="45" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I1" s="45"/>
       <c r="J1" s="45"/>
       <c r="K1" s="45"/>
-      <c r="L1" s="67" t="s">
-        <v>154</v>
-      </c>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
+      <c r="L1" s="70" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
     </row>
     <row r="2" spans="1:14 16384:16384" x14ac:dyDescent="0.2">
       <c r="A2" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="47" t="s">
         <v>135</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>136</v>
       </c>
       <c r="C2" s="46" t="s">
         <v>100</v>
@@ -18544,16 +18570,16 @@
         <v>66</v>
       </c>
       <c r="E2" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="G2" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="G2" s="46" t="s">
-        <v>139</v>
-      </c>
       <c r="H2" s="48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I2" s="46" t="s">
         <v>68</v>
@@ -18571,7 +18597,7 @@
         <v>64</v>
       </c>
       <c r="N2" s="46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:14 16384:16384" x14ac:dyDescent="0.2">
@@ -18631,7 +18657,7 @@
     <row r="4" spans="1:14 16384:16384" x14ac:dyDescent="0.2">
       <c r="A4" s="49"/>
       <c r="B4" s="50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C4" s="49">
         <f ca="1">AVERAGE(C5:INDIRECT("C"&amp;4+META!$B$2))</f>
@@ -18654,16 +18680,16 @@
         <v>0</v>
       </c>
       <c r="H4" s="55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I4" s="55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J4" s="55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K4" s="55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L4" s="59">
         <f>AVERAGE(L5:L221)</f>
@@ -18674,10 +18700,10 @@
         <v>0</v>
       </c>
       <c r="N4" s="61" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="XFD4" s="49" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:14 16384:16384" x14ac:dyDescent="0.2">
@@ -31421,22 +31447,22 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="68" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="69" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="72" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
       <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -31447,13 +31473,13 @@
         <v>71</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E2" s="46" t="s">
         <v>72</v>
       </c>
       <c r="F2" s="46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G2" s="46" t="s">
         <v>73</v>
@@ -31462,13 +31488,13 @@
         <v>71</v>
       </c>
       <c r="I2" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J2" s="46" t="s">
         <v>72</v>
       </c>
       <c r="K2" s="46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L2" s="53" t="s">
         <v>73</v>
@@ -31525,7 +31551,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4">
         <f ca="1">COUNT(BASELINE!$A$3:INDIRECT("BASELINE!A"&amp;META!$B$1))</f>
@@ -31574,7 +31600,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B5" s="5">
         <f ca="1">B3/B4</f>
@@ -31651,50 +31677,50 @@
     <col min="9" max="9" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="87" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="s">
+    <row r="1" spans="1:9" s="66" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="66" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="66" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="C1" s="66" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="D1" s="66" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="66" t="s">
         <v>191</v>
       </c>
-      <c r="D1" s="87" t="s">
-        <v>195</v>
-      </c>
-      <c r="E1" s="87" t="s">
-        <v>192</v>
-      </c>
-      <c r="F1" s="90" t="s">
+      <c r="F1" s="69" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1" s="69" t="s">
         <v>203</v>
       </c>
-      <c r="G1" s="90" t="s">
+      <c r="H1" s="66" t="s">
         <v>204</v>
       </c>
-      <c r="H1" s="87" t="s">
+      <c r="I1" s="66" t="s">
         <v>205</v>
-      </c>
-      <c r="I1" s="87" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="68">
+        <v>1000</v>
+      </c>
+      <c r="E2" t="s">
         <v>196</v>
-      </c>
-      <c r="B2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D2" s="89">
-        <v>1000</v>
-      </c>
-      <c r="E2" t="s">
-        <v>197</v>
       </c>
       <c r="F2" s="5">
         <f>IF(C2="Acquisition", IF(E2="Monthly", (D2*12)/52, IF(E2="Weekly", D2, 0)), 0)</f>
@@ -33582,7 +33608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726B1E90-CF35-6B44-A028-BC0D727236A8}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -33596,10 +33622,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="92"/>
+      <c r="B1" s="73"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -33651,7 +33677,7 @@
         <v>#N/A</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -33663,11 +33689,11 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="92" t="s">
-        <v>152</v>
-      </c>
-      <c r="B10" s="92"/>
-      <c r="C10" s="92"/>
+      <c r="A10" s="73" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
     </row>
     <row r="11" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
@@ -33747,11 +33773,11 @@
       <c r="B17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="92" t="s">
-        <v>156</v>
-      </c>
-      <c r="B18" s="92"/>
-      <c r="C18" s="92"/>
+      <c r="A18" s="73" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="73"/>
+      <c r="C18" s="73"/>
     </row>
     <row r="19" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
@@ -33777,7 +33803,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B21">
         <f ca="1">AVERAGE(INDIRECT("BASELINE!O3:O"&amp;META!B1))</f>
@@ -33793,10 +33819,10 @@
       <c r="B22" s="12"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="93" t="s">
-        <v>153</v>
-      </c>
-      <c r="B23" s="93"/>
+      <c r="A23" s="76" t="s">
+        <v>152</v>
+      </c>
+      <c r="B23" s="76"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -33808,24 +33834,24 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="94" t="s">
-        <v>202</v>
-      </c>
-      <c r="B26" s="91"/>
-      <c r="C26" s="91"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="91"/>
+      <c r="A26" s="74" t="s">
+        <v>201</v>
+      </c>
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
     </row>
     <row r="27" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>72</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>73</v>
@@ -33833,7 +33859,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B28" s="5">
         <f>SUMIF(TACTICS!B2:B104, $B$27, TACTICS!F2:F104)</f>
@@ -33854,7 +33880,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B29" s="5">
         <f>SUMIF(TACTICS!$B$2:$B$104, B$27, TACTICS!$G$2:$G$104)</f>
@@ -33875,7 +33901,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B30" s="5">
         <f>SUMIF(TACTICS!B2:B104, $B$27, TACTICS!H2:H104)</f>
@@ -33896,7 +33922,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B31" s="5">
         <f>SUMIF(TACTICS!$B$2:$B$104, B$27, TACTICS!$I$2:$I$104)</f>
@@ -33931,7 +33957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4156A3-96B9-DE41-91DB-F4C9577E214C}">
   <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="111" workbookViewId="0">
+    <sheetView zoomScale="111" workbookViewId="0">
       <selection activeCell="X40" sqref="X40"/>
     </sheetView>
   </sheetViews>
@@ -33961,34 +33987,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="77" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
     </row>
     <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -34046,28 +34072,28 @@
         <v>20</v>
       </c>
       <c r="S2" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="T2" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="U2" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="V2" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="W2" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="W2" s="11" t="s">
+      <c r="X2" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="Y2" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="Y2" s="11" t="s">
+      <c r="Z2" s="11" t="s">
         <v>164</v>
-      </c>
-      <c r="Z2" s="11" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -37662,8 +37688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCFA04E-CEAE-1D4C-9348-08755944D418}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37675,12 +37701,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="76"/>
+      <c r="B1" s="83"/>
       <c r="D1" s="49" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E1" s="49"/>
     </row>
@@ -37688,7 +37714,7 @@
       <c r="A2" s="8"/>
       <c r="B2" s="17"/>
       <c r="D2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E2" s="2" t="e">
         <f ca="1">INPUTS!B7</f>
@@ -37696,12 +37722,12 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="78"/>
+      <c r="B3" s="85"/>
       <c r="D3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E3" s="2" t="e">
         <f ca="1">E2-3</f>
@@ -37713,13 +37739,13 @@
         <v>59</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" t="s">
         <v>170</v>
-      </c>
-      <c r="E4" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -37730,10 +37756,10 @@
         <v>43542</v>
       </c>
       <c r="D5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E5" t="s">
         <v>172</v>
-      </c>
-      <c r="E5" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -37745,10 +37771,10 @@
         <v>#N/A</v>
       </c>
       <c r="D6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E6" t="s">
         <v>174</v>
-      </c>
-      <c r="E6" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -37760,10 +37786,10 @@
         <v>#N/A</v>
       </c>
       <c r="D7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E7" t="s">
         <v>176</v>
-      </c>
-      <c r="E7" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -37775,21 +37801,33 @@
         <v>1000</v>
       </c>
       <c r="D8" t="s">
+        <v>177</v>
+      </c>
+      <c r="E8" t="s">
         <v>178</v>
-      </c>
-      <c r="E8" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="21"/>
+      <c r="D9" s="94" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="80"/>
+      <c r="B10" s="87"/>
+      <c r="D10" s="94" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
@@ -37799,6 +37837,12 @@
         <f ca="1">INDIRECT("MODEL!N"&amp;E2)-MODEL!N3</f>
         <v>#N/A</v>
       </c>
+      <c r="D11" s="94" t="s">
+        <v>209</v>
+      </c>
+      <c r="E11" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -37808,6 +37852,12 @@
         <f ca="1">SUM(INDIRECT("MODEL!F4:F"&amp;E2))</f>
         <v>#N/A</v>
       </c>
+      <c r="D12" s="94" t="s">
+        <v>210</v>
+      </c>
+      <c r="E12" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
@@ -37817,6 +37867,12 @@
         <f ca="1">B12/B42</f>
         <v>#N/A</v>
       </c>
+      <c r="D13" s="94" t="s">
+        <v>211</v>
+      </c>
+      <c r="E13" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -37826,6 +37882,12 @@
         <f ca="1">SUM(INDIRECT("MODEL!K4:K"&amp;E2))</f>
         <v>#N/A</v>
       </c>
+      <c r="D14" s="94" t="s">
+        <v>212</v>
+      </c>
+      <c r="E14" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -37835,6 +37897,12 @@
         <f ca="1">SUM(INDIRECT("MODEL!L4:L"&amp;E2))</f>
         <v>#N/A</v>
       </c>
+      <c r="D15" s="94" t="s">
+        <v>213</v>
+      </c>
+      <c r="E15" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -37844,6 +37912,12 @@
         <f ca="1">B15/B17</f>
         <v>#N/A</v>
       </c>
+      <c r="D16" s="94" t="s">
+        <v>214</v>
+      </c>
+      <c r="E16" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
@@ -37886,10 +37960,10 @@
       <c r="B21" s="17"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="81" t="s">
+      <c r="A22" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="82"/>
+      <c r="B22" s="89"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
@@ -37941,10 +38015,10 @@
       <c r="B28" s="17"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="83" t="s">
+      <c r="A29" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="84"/>
+      <c r="B29" s="91"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
@@ -38117,7 +38191,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>41</v>
       </c>
@@ -38126,65 +38200,53 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="17"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="85" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="B51" s="86"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B51" s="93"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B52" s="24" t="e">
-        <f ca="1">SUM(INDIRECT("MODEL!"&amp;C52&amp;"4:"&amp;C52&amp;$E$2))</f>
+        <f ca="1">SUM(INDIRECT("MODEL!"&amp;E9&amp;"4:"&amp;E9&amp;$E$2))+INPUTS!C30</f>
         <v>#N/A</v>
       </c>
-      <c r="C52" s="66" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B53" s="24" t="e">
-        <f t="shared" ref="B53:B55" ca="1" si="0">SUM(INDIRECT("MODEL!"&amp;C53&amp;"4:"&amp;C53&amp;$E$2))</f>
+        <f ca="1">SUM(INDIRECT("MODEL!"&amp;E10&amp;"4:"&amp;E10&amp;$E$2))+INPUTS!D30</f>
         <v>#N/A</v>
       </c>
-      <c r="C53" s="66" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B54" s="24" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">SUM(INDIRECT("MODEL!"&amp;E11&amp;"4:"&amp;E11&amp;$E$2))+INPUTS!E30</f>
         <v>#N/A</v>
       </c>
-      <c r="C54" s="66" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B55" s="24" t="e">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">SUM(INDIRECT("MODEL!"&amp;E12&amp;"4:"&amp;E12&amp;$E$2))+INPUTS!B30</f>
         <v>#N/A</v>
       </c>
-      <c r="C55" s="66" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>46</v>
       </c>
@@ -38193,7 +38255,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>47</v>
       </c>
@@ -38202,7 +38264,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>48</v>
       </c>
@@ -38211,62 +38273,50 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="B59" s="24"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="71" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="B60" s="72"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B60" s="79"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B61" s="24" t="e">
-        <f ca="1">SUM(INDIRECT("MODEL!"&amp;C61&amp;"4:"&amp;C61&amp;$E$2))</f>
+        <f ca="1">SUM(INDIRECT("MODEL!"&amp;E13&amp;"4:"&amp;E13&amp;$E$2))+INPUTS!C31</f>
         <v>#N/A</v>
       </c>
-      <c r="C61" s="66" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B62" s="24" t="e">
-        <f t="shared" ref="B62:B64" ca="1" si="1">SUM(INDIRECT("MODEL!"&amp;C62&amp;"4:"&amp;C62&amp;$E$2))</f>
+        <f ca="1">SUM(INDIRECT("MODEL!"&amp;E14&amp;"4:"&amp;E14&amp;$E$2))+INPUTS!D31</f>
         <v>#N/A</v>
       </c>
-      <c r="C62" s="66" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B63" s="24" t="e">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">SUM(INDIRECT("MODEL!"&amp;E15&amp;"4:"&amp;E15&amp;$E$2))+INPUTS!E31</f>
         <v>#N/A</v>
       </c>
-      <c r="C63" s="66" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B64" s="24" t="e">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">SUM(INDIRECT("MODEL!"&amp;E16&amp;"4:"&amp;E16&amp;$E$2))+INPUTS!B31</f>
         <v>#N/A</v>
-      </c>
-      <c r="C64" s="66" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -38301,10 +38351,10 @@
       <c r="B68" s="24"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="73" t="s">
+      <c r="A69" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="B69" s="74"/>
+      <c r="B69" s="81"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
@@ -38353,7 +38403,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38367,7 +38417,7 @@
         <v>106</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated deadline and run-rate
</commit_message>
<xml_diff>
--- a/xls/templates/deadline-driven-template.xlsx
+++ b/xls/templates/deadline-driven-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toddcullen/Projects/remarkably/xls/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BFF9DB9-8A2B-174A-B728-025123830A08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D40147-9516-E144-89FB-BF6388703390}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="38400" windowHeight="21060" activeTab="7" xr2:uid="{37D2F886-AD7C-B54B-8546-6E8B72F70745}"/>
+    <workbookView xWindow="28000" yWindow="460" windowWidth="33600" windowHeight="20460" activeTab="3" xr2:uid="{37D2F886-AD7C-B54B-8546-6E8B72F70745}"/>
   </bookViews>
   <sheets>
     <sheet name="CONSTANTS" sheetId="12" r:id="rId1"/>
@@ -1144,6 +1144,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="19"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="11" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1215,9 +1218,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -18550,11 +18550,11 @@
       <c r="I1" s="45"/>
       <c r="J1" s="45"/>
       <c r="K1" s="45"/>
-      <c r="L1" s="70" t="s">
+      <c r="L1" s="71" t="s">
         <v>153</v>
       </c>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
     </row>
     <row r="2" spans="1:14 16384:16384" x14ac:dyDescent="0.2">
       <c r="A2" s="47" t="s">
@@ -31427,8 +31427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D531062B-9844-554D-B6BC-FF56937D80E1}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31449,20 +31449,20 @@
       <c r="B1" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="72" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="72" t="s">
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="73" t="s">
         <v>140</v>
       </c>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
       <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -31521,11 +31521,11 @@
         <v>0</v>
       </c>
       <c r="F3" s="5">
-        <f ca="1">SUM(BASELINE!U$3:INDIRECT("BASELINE!T"&amp;META!$B$1))</f>
+        <f ca="1">SUM(BASELINE!U$3:INDIRECT("BASELINE!U"&amp;META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="G3" s="5">
-        <f ca="1">SUM(BASELINE!V$3:INDIRECT("BASELINE!T"&amp;META!$B$1))</f>
+        <f ca="1">SUM(BASELINE!V$3:INDIRECT("BASELINE!V"&amp;META!$B$1))</f>
         <v>0</v>
       </c>
       <c r="H3" s="5">
@@ -33609,7 +33609,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33622,10 +33622,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="73"/>
+      <c r="B1" s="74"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -33673,7 +33673,7 @@
         <v>102</v>
       </c>
       <c r="B7" s="64" t="e">
-        <f ca="1">ROW(INDEX(MODEL!O4:O43,MATCH(TRUE,INDEX(MODEL!O4:O43&gt;B5,0),)))</f>
+        <f ca="1">ROW(INDEX(MODEL!O4:O43,MATCH(TRUE,INDEX(MODEL!O4:O43&gt;=B5,0),)))</f>
         <v>#N/A</v>
       </c>
       <c r="C7" t="s">
@@ -33689,11 +33689,11 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="74" t="s">
         <v>151</v>
       </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
     </row>
     <row r="11" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
@@ -33773,11 +33773,11 @@
       <c r="B17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="74" t="s">
         <v>155</v>
       </c>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="74"/>
     </row>
     <row r="19" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
@@ -33819,10 +33819,10 @@
       <c r="B22" s="12"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="76" t="s">
+      <c r="A23" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="B23" s="76"/>
+      <c r="B23" s="77"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -33834,13 +33834,13 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="75" t="s">
         <v>201</v>
       </c>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
     </row>
     <row r="27" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
@@ -33957,8 +33957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4156A3-96B9-DE41-91DB-F4C9577E214C}">
   <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0">
-      <selection activeCell="X40" sqref="X40"/>
+    <sheetView topLeftCell="M1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="S39" sqref="S39:T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33987,34 +33987,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="78" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
     </row>
     <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -37688,8 +37688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCFA04E-CEAE-1D4C-9348-08755944D418}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37701,10 +37701,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="83"/>
+      <c r="B1" s="84"/>
       <c r="D1" s="49" t="s">
         <v>165</v>
       </c>
@@ -37722,10 +37722,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="85"/>
+      <c r="B3" s="86"/>
       <c r="D3" t="s">
         <v>168</v>
       </c>
@@ -37767,7 +37767,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="18" t="e">
-        <f ca="1">INDIRECT("MODEL!A"&amp;INPUTS!B7)</f>
+        <f ca="1">INDIRECT("MODEL!A"&amp;INPUTS!B7)+6</f>
         <v>#N/A</v>
       </c>
       <c r="D6" t="s">
@@ -37810,7 +37810,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="21"/>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="70" t="s">
         <v>207</v>
       </c>
       <c r="E9" t="s">
@@ -37818,11 +37818,11 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="86" t="s">
+      <c r="A10" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="87"/>
-      <c r="D10" s="94" t="s">
+      <c r="B10" s="88"/>
+      <c r="D10" s="70" t="s">
         <v>208</v>
       </c>
       <c r="E10" t="s">
@@ -37837,7 +37837,7 @@
         <f ca="1">INDIRECT("MODEL!N"&amp;E2)-MODEL!N3</f>
         <v>#N/A</v>
       </c>
-      <c r="D11" s="94" t="s">
+      <c r="D11" s="70" t="s">
         <v>209</v>
       </c>
       <c r="E11" t="s">
@@ -37852,7 +37852,7 @@
         <f ca="1">SUM(INDIRECT("MODEL!F4:F"&amp;E2))</f>
         <v>#N/A</v>
       </c>
-      <c r="D12" s="94" t="s">
+      <c r="D12" s="70" t="s">
         <v>210</v>
       </c>
       <c r="E12" t="s">
@@ -37867,7 +37867,7 @@
         <f ca="1">B12/B42</f>
         <v>#N/A</v>
       </c>
-      <c r="D13" s="94" t="s">
+      <c r="D13" s="70" t="s">
         <v>211</v>
       </c>
       <c r="E13" t="s">
@@ -37882,7 +37882,7 @@
         <f ca="1">SUM(INDIRECT("MODEL!K4:K"&amp;E2))</f>
         <v>#N/A</v>
       </c>
-      <c r="D14" s="94" t="s">
+      <c r="D14" s="70" t="s">
         <v>212</v>
       </c>
       <c r="E14" t="s">
@@ -37897,7 +37897,7 @@
         <f ca="1">SUM(INDIRECT("MODEL!L4:L"&amp;E2))</f>
         <v>#N/A</v>
       </c>
-      <c r="D15" s="94" t="s">
+      <c r="D15" s="70" t="s">
         <v>213</v>
       </c>
       <c r="E15" t="s">
@@ -37909,10 +37909,10 @@
         <v>10</v>
       </c>
       <c r="B16" s="19" t="e">
-        <f ca="1">B15/B17</f>
+        <f ca="1">B14/B17</f>
         <v>#N/A</v>
       </c>
-      <c r="D16" s="94" t="s">
+      <c r="D16" s="70" t="s">
         <v>214</v>
       </c>
       <c r="E16" t="s">
@@ -37923,8 +37923,8 @@
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="17" t="e">
-        <f ca="1">B18+B15</f>
+      <c r="B17" s="23" t="e">
+        <f ca="1">B18+B14</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -37960,10 +37960,10 @@
       <c r="B21" s="17"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="88" t="s">
+      <c r="A22" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="89"/>
+      <c r="B22" s="90"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
@@ -38015,10 +38015,10 @@
       <c r="B28" s="17"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="90" t="s">
+      <c r="A29" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="91"/>
+      <c r="B29" s="92"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
@@ -38205,10 +38205,10 @@
       <c r="B50" s="17"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="92" t="s">
+      <c r="A51" s="93" t="s">
         <v>74</v>
       </c>
-      <c r="B51" s="93"/>
+      <c r="B51" s="94"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
@@ -38278,10 +38278,10 @@
       <c r="B59" s="24"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="78" t="s">
+      <c r="A60" s="79" t="s">
         <v>75</v>
       </c>
-      <c r="B60" s="79"/>
+      <c r="B60" s="80"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
@@ -38351,10 +38351,10 @@
       <c r="B68" s="24"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="80" t="s">
+      <c r="A69" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="B69" s="81"/>
+      <c r="B69" s="82"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">

</xml_diff>

<commit_message>
Implement modeling option importer. Implement require_complete(...)
</commit_message>
<xml_diff>
--- a/xls/templates/deadline-driven-template.xlsx
+++ b/xls/templates/deadline-driven-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toddcullen/Projects/remarkably/xls/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/dev/psl/remarkably/xls/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D40147-9516-E144-89FB-BF6388703390}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8FED2A-D7BA-F94B-9B9A-A6D99E682675}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28000" yWindow="460" windowWidth="33600" windowHeight="20460" activeTab="3" xr2:uid="{37D2F886-AD7C-B54B-8546-6E8B72F70745}"/>
+    <workbookView xWindow="68880" yWindow="15260" windowWidth="28640" windowHeight="17380" activeTab="8" xr2:uid="{37D2F886-AD7C-B54B-8546-6E8B72F70745}"/>
   </bookViews>
   <sheets>
     <sheet name="CONSTANTS" sheetId="12" r:id="rId1"/>
@@ -660,9 +660,6 @@
     <t>Ret Setup Cost</t>
   </si>
   <si>
-    <t>deadline_model</t>
-  </si>
-  <si>
     <t>Acq DC</t>
   </si>
   <si>
@@ -685,6 +682,9 @@
   </si>
   <si>
     <t>Ret RB</t>
+  </si>
+  <si>
+    <t>model</t>
   </si>
 </sst>
 </file>
@@ -31427,7 +31427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D531062B-9844-554D-B6BC-FF56937D80E1}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -37811,7 +37811,7 @@
       <c r="A9" s="3"/>
       <c r="B9" s="21"/>
       <c r="D9" s="70" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E9" t="s">
         <v>179</v>
@@ -37823,7 +37823,7 @@
       </c>
       <c r="B10" s="88"/>
       <c r="D10" s="70" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E10" t="s">
         <v>180</v>
@@ -37838,7 +37838,7 @@
         <v>#N/A</v>
       </c>
       <c r="D11" s="70" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E11" t="s">
         <v>181</v>
@@ -37853,7 +37853,7 @@
         <v>#N/A</v>
       </c>
       <c r="D12" s="70" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E12" t="s">
         <v>182</v>
@@ -37868,7 +37868,7 @@
         <v>#N/A</v>
       </c>
       <c r="D13" s="70" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E13" t="s">
         <v>184</v>
@@ -37883,7 +37883,7 @@
         <v>#N/A</v>
       </c>
       <c r="D14" s="70" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E14" t="s">
         <v>185</v>
@@ -37898,7 +37898,7 @@
         <v>#N/A</v>
       </c>
       <c r="D15" s="70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E15" t="s">
         <v>186</v>
@@ -37913,7 +37913,7 @@
         <v>#N/A</v>
       </c>
       <c r="D16" s="70" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E16" t="s">
         <v>183</v>
@@ -38402,8 +38402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0220B30-5172-8F43-B617-05CBEB835057}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -38417,7 +38417,7 @@
         <v>106</v>
       </c>
       <c r="B1" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix spelling error in OUTPUT headers
</commit_message>
<xml_diff>
--- a/xls/templates/deadline-driven-template.xlsx
+++ b/xls/templates/deadline-driven-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/dev/psl/remarkably/xls/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8FED2A-D7BA-F94B-9B9A-A6D99E682675}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C38427-49A2-7746-8643-CE44C1E71212}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68880" yWindow="15260" windowWidth="28640" windowHeight="17380" activeTab="8" xr2:uid="{37D2F886-AD7C-B54B-8546-6E8B72F70745}"/>
+    <workbookView xWindow="68880" yWindow="15260" windowWidth="28640" windowHeight="17380" activeTab="7" xr2:uid="{37D2F886-AD7C-B54B-8546-6E8B72F70745}"/>
   </bookViews>
   <sheets>
     <sheet name="CONSTANTS" sheetId="12" r:id="rId1"/>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>EXE 4 Week</t>
-  </si>
-  <si>
-    <t>Acquistion Demand Creation</t>
   </si>
   <si>
     <t>Acquisition Leasing Enablement</t>
@@ -685,6 +682,9 @@
   </si>
   <si>
     <t>model</t>
+  </si>
+  <si>
+    <t>Acquisition Demand Creation</t>
   </si>
 </sst>
 </file>
@@ -1566,48 +1566,48 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="67" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="C1" s="67" t="s">
         <v>190</v>
-      </c>
-      <c r="C1" s="67" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1630,7 +1630,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1">
         <v>12</v>
@@ -1638,7 +1638,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2">
         <f>B1-2</f>
@@ -1679,7 +1679,7 @@
       <c r="A1" s="28"/>
       <c r="B1" s="28"/>
       <c r="C1" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D1" s="30"/>
       <c r="E1" s="30"/>
@@ -1690,24 +1690,24 @@
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
       <c r="L1" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M1" s="32"/>
       <c r="N1" s="32"/>
       <c r="O1" s="32"/>
       <c r="P1" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q1" s="34"/>
       <c r="R1" s="34"/>
       <c r="S1" s="35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="T1" s="36"/>
       <c r="U1" s="36"/>
       <c r="V1" s="36"/>
       <c r="W1" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="X1" s="38"/>
       <c r="Y1" s="38"/>
@@ -1721,37 +1721,37 @@
         <v>1</v>
       </c>
       <c r="C2" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="E2" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="F2" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="G2" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="H2" s="41" t="s">
         <v>117</v>
-      </c>
-      <c r="H2" s="41" t="s">
-        <v>118</v>
       </c>
       <c r="I2" s="41" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="K2" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="L2" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="M2" s="41" t="s">
         <v>121</v>
-      </c>
-      <c r="M2" s="41" t="s">
-        <v>122</v>
       </c>
       <c r="N2" s="41" t="s">
         <v>16</v>
@@ -1760,37 +1760,37 @@
         <v>17</v>
       </c>
       <c r="P2" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q2" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="Q2" s="41" t="s">
-        <v>88</v>
-      </c>
       <c r="R2" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="S2" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="S2" s="42" t="s">
+      <c r="T2" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="T2" s="43" t="s">
+      <c r="U2" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="U2" s="43" t="s">
+      <c r="V2" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="V2" s="43" t="s">
+      <c r="W2" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="W2" s="42" t="s">
+      <c r="X2" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="X2" s="43" t="s">
+      <c r="Y2" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="Y2" s="43" t="s">
+      <c r="Z2" s="43" t="s">
         <v>130</v>
-      </c>
-      <c r="Z2" s="43" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
@@ -18538,72 +18538,72 @@
       <c r="A1" s="47"/>
       <c r="B1" s="47"/>
       <c r="C1" s="51" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
       <c r="G1" s="51"/>
       <c r="H1" s="45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I1" s="45"/>
       <c r="J1" s="45"/>
       <c r="K1" s="45"/>
       <c r="L1" s="71" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M1" s="71"/>
       <c r="N1" s="71"/>
     </row>
     <row r="2" spans="1:14 16384:16384" x14ac:dyDescent="0.2">
       <c r="A2" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="C2" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="46" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="46" t="s">
+      <c r="F2" s="46" t="s">
         <v>136</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="G2" s="46" t="s">
         <v>137</v>
       </c>
-      <c r="G2" s="46" t="s">
-        <v>138</v>
-      </c>
       <c r="H2" s="48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I2" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="K2" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="46" t="s">
-        <v>70</v>
-      </c>
       <c r="L2" s="56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M2" s="56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N2" s="46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:14 16384:16384" x14ac:dyDescent="0.2">
       <c r="A3" s="49"/>
       <c r="B3" s="50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="49">
         <f>SUM(C5:C221)</f>
@@ -18657,7 +18657,7 @@
     <row r="4" spans="1:14 16384:16384" x14ac:dyDescent="0.2">
       <c r="A4" s="49"/>
       <c r="B4" s="50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C4" s="49">
         <f ca="1">AVERAGE(C5:INDIRECT("C"&amp;4+META!$B$2))</f>
@@ -18680,16 +18680,16 @@
         <v>0</v>
       </c>
       <c r="H4" s="55" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I4" s="55" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J4" s="55" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K4" s="55" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L4" s="59">
         <f>AVERAGE(L5:L221)</f>
@@ -18700,10 +18700,10 @@
         <v>0</v>
       </c>
       <c r="N4" s="61" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="XFD4" s="49" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:14 16384:16384" x14ac:dyDescent="0.2">
@@ -31447,17 +31447,17 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="72" t="s">
         <v>143</v>
-      </c>
-      <c r="C1" s="72" t="s">
-        <v>144</v>
       </c>
       <c r="D1" s="72"/>
       <c r="E1" s="72"/>
       <c r="F1" s="72"/>
       <c r="G1" s="72"/>
       <c r="H1" s="73" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I1" s="73"/>
       <c r="J1" s="73"/>
@@ -31467,42 +31467,42 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="F2" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="K2" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="L2" s="53" t="s">
         <v>72</v>
-      </c>
-      <c r="F2" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="G2" s="46" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="I2" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="J2" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="K2" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="L2" s="53" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="5">
         <f ca="1">C3+H3</f>
@@ -31551,7 +31551,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4">
         <f ca="1">COUNT(BASELINE!$A$3:INDIRECT("BASELINE!A"&amp;META!$B$1))</f>
@@ -31600,7 +31600,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="5">
         <f ca="1">B3/B4</f>
@@ -31679,48 +31679,48 @@
   <sheetData>
     <row r="1" spans="1:9" s="66" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="66" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="66" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="C1" s="66" t="s">
         <v>189</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="D1" s="66" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" s="66" t="s">
         <v>190</v>
       </c>
-      <c r="D1" s="66" t="s">
-        <v>194</v>
-      </c>
-      <c r="E1" s="66" t="s">
-        <v>191</v>
-      </c>
       <c r="F1" s="69" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" s="69" t="s">
         <v>202</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="H1" s="66" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="I1" s="66" t="s">
         <v>204</v>
-      </c>
-      <c r="I1" s="66" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D2" s="68">
         <v>1000</v>
       </c>
       <c r="E2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F2" s="5">
         <f>IF(C2="Acquisition", IF(E2="Monthly", (D2*12)/52, IF(E2="Weekly", D2, 0)), 0)</f>
@@ -33623,7 +33623,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="74" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="74"/>
     </row>
@@ -33637,7 +33637,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="14">
         <f ca="1">INDIRECT("BASELINE!M"&amp;META!B1)</f>
@@ -33646,7 +33646,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="14">
         <v>253</v>
@@ -33654,7 +33654,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="65">
         <v>0.9</v>
@@ -33662,7 +33662,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="14">
         <v>250</v>
@@ -33670,14 +33670,14 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="64" t="e">
         <f ca="1">ROW(INDEX(MODEL!O4:O43,MATCH(TRUE,INDEX(MODEL!O4:O43&gt;=B5,0),)))</f>
         <v>#N/A</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -33690,7 +33690,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10" s="74"/>
       <c r="C10" s="74"/>
@@ -33698,15 +33698,15 @@
     <row r="11" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="7">
         <f>FUNNEL!H3</f>
@@ -33719,7 +33719,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" s="7">
         <f>FUNNEL!I3</f>
@@ -33732,7 +33732,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="7">
         <f>FUNNEL!J3</f>
@@ -33745,7 +33745,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="7">
         <f>FUNNEL!K3</f>
@@ -33758,7 +33758,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="7">
         <f>FUNNEL!N3</f>
@@ -33774,7 +33774,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="74" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B18" s="74"/>
       <c r="C18" s="74"/>
@@ -33782,15 +33782,15 @@
     <row r="19" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20">
         <f ca="1">FUNNEL!C4</f>
@@ -33803,7 +33803,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B21">
         <f ca="1">AVERAGE(INDIRECT("BASELINE!O3:O"&amp;META!B1))</f>
@@ -33820,13 +33820,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="77" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23" s="77"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B24" s="15">
         <f ca="1">COUNT(INDIRECT("MODEL!A4:A"&amp;B7))</f>
@@ -33835,7 +33835,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="75" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B26" s="76"/>
       <c r="C26" s="76"/>
@@ -33845,21 +33845,21 @@
     <row r="27" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="E27" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B28" s="5">
         <f>SUMIF(TACTICS!B2:B104, $B$27, TACTICS!F2:F104)</f>
@@ -33880,7 +33880,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B29" s="5">
         <f>SUMIF(TACTICS!$B$2:$B$104, B$27, TACTICS!$G$2:$G$104)</f>
@@ -33901,7 +33901,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B30" s="5">
         <f>SUMIF(TACTICS!B2:B104, $B$27, TACTICS!H2:H104)</f>
@@ -33922,7 +33922,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B31" s="5">
         <f>SUMIF(TACTICS!$B$2:$B$104, B$27, TACTICS!$I$2:$I$104)</f>
@@ -33988,7 +33988,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="78" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="78"/>
       <c r="C1" s="78"/>
@@ -34018,87 +34018,87 @@
     </row>
     <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>88</v>
-      </c>
       <c r="D2" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>61</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>62</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N2" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O2" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="P2" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="R2" s="11" t="s">
         <v>20</v>
       </c>
       <c r="S2" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="T2" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="T2" s="11" t="s">
+      <c r="U2" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="U2" s="11" t="s">
+      <c r="V2" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="V2" s="11" t="s">
+      <c r="W2" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="W2" s="11" t="s">
+      <c r="X2" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="Y2" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="Y2" s="11" t="s">
+      <c r="Z2" s="11" t="s">
         <v>163</v>
-      </c>
-      <c r="Z2" s="11" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N3" s="1">
         <f>INPUTS!B4</f>
@@ -37688,8 +37688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCFA04E-CEAE-1D4C-9348-08755944D418}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -37702,11 +37702,11 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="83" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="84"/>
       <c r="D1" s="49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E1" s="49"/>
     </row>
@@ -37714,7 +37714,7 @@
       <c r="A2" s="8"/>
       <c r="B2" s="17"/>
       <c r="D2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E2" s="2" t="e">
         <f ca="1">INPUTS!B7</f>
@@ -37723,11 +37723,11 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="85" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="86"/>
       <c r="D3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E3" s="2" t="e">
         <f ca="1">E2-3</f>
@@ -37736,16 +37736,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" t="s">
         <v>169</v>
-      </c>
-      <c r="E4" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -37756,10 +37756,10 @@
         <v>43542</v>
       </c>
       <c r="D5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" t="s">
         <v>171</v>
-      </c>
-      <c r="E5" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -37771,10 +37771,10 @@
         <v>#N/A</v>
       </c>
       <c r="D6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" t="s">
         <v>173</v>
-      </c>
-      <c r="E6" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -37786,10 +37786,10 @@
         <v>#N/A</v>
       </c>
       <c r="D7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" t="s">
         <v>175</v>
-      </c>
-      <c r="E7" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -37801,20 +37801,20 @@
         <v>1000</v>
       </c>
       <c r="D8" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" t="s">
         <v>177</v>
-      </c>
-      <c r="E8" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="21"/>
       <c r="D9" s="70" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -37823,10 +37823,10 @@
       </c>
       <c r="B10" s="88"/>
       <c r="D10" s="70" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -37838,10 +37838,10 @@
         <v>#N/A</v>
       </c>
       <c r="D11" s="70" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -37853,10 +37853,10 @@
         <v>#N/A</v>
       </c>
       <c r="D12" s="70" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -37868,10 +37868,10 @@
         <v>#N/A</v>
       </c>
       <c r="D13" s="70" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -37883,10 +37883,10 @@
         <v>#N/A</v>
       </c>
       <c r="D14" s="70" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -37898,10 +37898,10 @@
         <v>#N/A</v>
       </c>
       <c r="D15" s="70" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -37913,10 +37913,10 @@
         <v>#N/A</v>
       </c>
       <c r="D16" s="70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -38206,13 +38206,13 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="93" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B51" s="94"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>42</v>
+        <v>214</v>
       </c>
       <c r="B52" s="24" t="e">
         <f ca="1">SUM(INDIRECT("MODEL!"&amp;E9&amp;"4:"&amp;E9&amp;$E$2))+INPUTS!C30</f>
@@ -38221,7 +38221,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B53" s="24" t="e">
         <f ca="1">SUM(INDIRECT("MODEL!"&amp;E10&amp;"4:"&amp;E10&amp;$E$2))+INPUTS!D30</f>
@@ -38230,7 +38230,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B54" s="24" t="e">
         <f ca="1">SUM(INDIRECT("MODEL!"&amp;E11&amp;"4:"&amp;E11&amp;$E$2))+INPUTS!E30</f>
@@ -38239,7 +38239,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B55" s="24" t="e">
         <f ca="1">SUM(INDIRECT("MODEL!"&amp;E12&amp;"4:"&amp;E12&amp;$E$2))+INPUTS!B30</f>
@@ -38248,7 +38248,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B56" s="24" t="e">
         <f ca="1">SUM(B52:B55)</f>
@@ -38257,7 +38257,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B57" s="17" t="e">
         <f ca="1">ROUND(B58/B56,0)</f>
@@ -38266,7 +38266,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B58" s="24" t="e">
         <f ca="1">B23*(B8*12)</f>
@@ -38279,13 +38279,13 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="79" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B60" s="80"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B61" s="24" t="e">
         <f ca="1">SUM(INDIRECT("MODEL!"&amp;E13&amp;"4:"&amp;E13&amp;$E$2))+INPUTS!C31</f>
@@ -38294,7 +38294,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B62" s="24" t="e">
         <f ca="1">SUM(INDIRECT("MODEL!"&amp;E14&amp;"4:"&amp;E14&amp;$E$2))+INPUTS!D31</f>
@@ -38303,7 +38303,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B63" s="24" t="e">
         <f ca="1">SUM(INDIRECT("MODEL!"&amp;E15&amp;"4:"&amp;E15&amp;$E$2))+INPUTS!E31</f>
@@ -38312,7 +38312,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B64" s="24" t="e">
         <f ca="1">SUM(INDIRECT("MODEL!"&amp;E16&amp;"4:"&amp;E16&amp;$E$2))+INPUTS!B31</f>
@@ -38321,7 +38321,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B65" s="24" t="e">
         <f ca="1">SUM(B61:B64)</f>
@@ -38330,7 +38330,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B66" s="17" t="e">
         <f ca="1">ROUND(B67/B65,0)</f>
@@ -38339,7 +38339,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B67" s="24" t="e">
         <f ca="1">B15*(B8*12)</f>
@@ -38352,13 +38352,13 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="81" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B69" s="82"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B70" s="24" t="e">
         <f ca="1">B65+B56</f>
@@ -38367,7 +38367,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B71" s="17" t="e">
         <f ca="1">ROUND(B72/B70,0)</f>
@@ -38376,7 +38376,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B72" s="26" t="e">
         <f ca="1">B67+B58</f>
@@ -38402,7 +38402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0220B30-5172-8F43-B617-05CBEB835057}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -38414,15 +38414,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>

</xml_diff>